<commit_message>
add solver/GPT optimization result in excel format
</commit_message>
<xml_diff>
--- a/result/GPT/sat/gpt_sat_result.xlsx
+++ b/result/GPT/sat/gpt_sat_result.xlsx
@@ -8,14 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/watsonhuang/Desktop/OSU/2025_Spring/CS 517/project/CS517-Final-Project/result/GPT/sat/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18B077DA-2CB6-8D47-BBC2-F64FD62423CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E8CA95C-1279-ED43-94A0-CF97A3F96CE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25600" yWindow="500" windowWidth="25600" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -704,10 +717,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C101"/>
+  <dimension ref="A1:C102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J47" sqref="J47"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C103" sqref="C103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1828,6 +1841,12 @@
         <v>80</v>
       </c>
     </row>
+    <row r="102" spans="1:3">
+      <c r="C102">
+        <f>AVERAGE(C2:C101)</f>
+        <v>89.34</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>